<commit_message>
Atualizadas durante testes de atuma~
</commit_message>
<xml_diff>
--- a/Data/g18.4.xlsx
+++ b/Data/g18.4.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1.204356017730487</v>
+        <v>1.204507731023762</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1.136989188371146</v>
+        <v>1.136973218646514</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.9805078283825769</v>
+        <v>0.9804530571292559</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.064575761022137</v>
+        <v>1.065176199645811</v>
       </c>
     </row>
     <row r="23">
@@ -777,22 +777,22 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.8020661872586382</v>
+        <v>1.087798046816562</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>01/01/2001</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.4772744654469883</v>
+        <v>0.3004981230324768</v>
       </c>
     </row>
     <row r="25">
@@ -803,11 +803,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>01/01/2002</t>
+          <t>01/01/2001</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.5532575945051468</v>
+        <v>0.4772744654469883</v>
       </c>
     </row>
     <row r="26">
@@ -818,11 +818,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>01/01/2003</t>
+          <t>01/01/2002</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.6204436706082329</v>
+        <v>0.5532575945051468</v>
       </c>
     </row>
     <row r="27">
@@ -833,11 +833,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>01/01/2004</t>
+          <t>01/01/2003</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.6269770215579353</v>
+        <v>0.6204436706082329</v>
       </c>
     </row>
     <row r="28">
@@ -848,11 +848,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>01/01/2005</t>
+          <t>01/01/2004</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.5949981691616898</v>
+        <v>0.6269770215579353</v>
       </c>
     </row>
     <row r="29">
@@ -863,11 +863,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>01/01/2006</t>
+          <t>01/01/2005</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.5419991935493135</v>
+        <v>0.5949981691616898</v>
       </c>
     </row>
     <row r="30">
@@ -878,11 +878,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>01/01/2007</t>
+          <t>01/01/2006</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.5858672095479524</v>
+        <v>0.5419991935493135</v>
       </c>
     </row>
     <row r="31">
@@ -893,11 +893,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>01/01/2008</t>
+          <t>01/01/2007</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.4859552888009054</v>
+        <v>0.5858672095479524</v>
       </c>
     </row>
     <row r="32">
@@ -908,11 +908,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>01/01/2009</t>
+          <t>01/01/2008</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.5531732981338393</v>
+        <v>0.4859552888009054</v>
       </c>
     </row>
     <row r="33">
@@ -923,11 +923,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>01/01/2010</t>
+          <t>01/01/2009</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.6577759822211939</v>
+        <v>0.5531732981338393</v>
       </c>
     </row>
     <row r="34">
@@ -938,11 +938,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>01/01/2011</t>
+          <t>01/01/2010</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.5229696404338543</v>
+        <v>0.6577759822211939</v>
       </c>
     </row>
     <row r="35">
@@ -953,11 +953,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
+          <t>01/01/2011</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1.874680179165634</v>
+        <v>0.5229696404338543</v>
       </c>
     </row>
     <row r="36">
@@ -968,11 +968,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
+          <t>01/01/2012</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2.133323612104753</v>
+        <v>1.874680179165634</v>
       </c>
     </row>
     <row r="37">
@@ -983,11 +983,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
+          <t>01/01/2013</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2.124534468979905</v>
+        <v>2.133323612104753</v>
       </c>
     </row>
     <row r="38">
@@ -998,11 +998,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
+          <t>01/01/2014</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1.444567115074851</v>
+        <v>2.124534468979905</v>
       </c>
     </row>
     <row r="39">
@@ -1013,11 +1013,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1.511515509064918</v>
+        <v>1.444567115074851</v>
       </c>
     </row>
     <row r="40">
@@ -1028,11 +1028,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1.44488291740586</v>
+        <v>1.511515509064918</v>
       </c>
     </row>
     <row r="41">
@@ -1043,11 +1043,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.372616737909732</v>
+        <v>1.44488291740586</v>
       </c>
     </row>
     <row r="42">
@@ -1058,11 +1058,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1.256453021277189</v>
+        <v>1.374213316911246</v>
       </c>
     </row>
     <row r="43">
@@ -1073,11 +1073,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1.07011495142484</v>
+        <v>1.256496275158019</v>
       </c>
     </row>
     <row r="44">
@@ -1088,11 +1088,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1.16655971494119</v>
+        <v>1.06910676406558</v>
       </c>
     </row>
     <row r="45">
@@ -1103,41 +1103,41 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.8973753371739895</v>
+        <v>1.166474645942877</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>01/01/2001</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.2340698640198239</v>
+        <v>1.207480173827043</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>01/01/2002</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.39975420518465</v>
+        <v>0.322157260470111</v>
       </c>
     </row>
     <row r="48">
@@ -1148,11 +1148,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>01/01/2003</t>
+          <t>01/01/2001</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.5628238604846239</v>
+        <v>0.2340698640198239</v>
       </c>
     </row>
     <row r="49">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>01/01/2004</t>
+          <t>01/01/2002</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.4621264110910339</v>
+        <v>0.39975420518465</v>
       </c>
     </row>
     <row r="50">
@@ -1178,11 +1178,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>01/01/2005</t>
+          <t>01/01/2003</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.5388747331451003</v>
+        <v>0.5628238604846239</v>
       </c>
     </row>
     <row r="51">
@@ -1193,11 +1193,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>01/01/2006</t>
+          <t>01/01/2004</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.4420086778692693</v>
+        <v>0.4621264110910339</v>
       </c>
     </row>
     <row r="52">
@@ -1208,11 +1208,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>01/01/2007</t>
+          <t>01/01/2005</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.4434061928072969</v>
+        <v>0.5388747331451003</v>
       </c>
     </row>
     <row r="53">
@@ -1223,11 +1223,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>01/01/2008</t>
+          <t>01/01/2006</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.3467491695790255</v>
+        <v>0.4420086778692693</v>
       </c>
     </row>
     <row r="54">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>01/01/2009</t>
+          <t>01/01/2007</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.4085367151094751</v>
+        <v>0.4434061928072969</v>
       </c>
     </row>
     <row r="55">
@@ -1253,11 +1253,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>01/01/2010</t>
+          <t>01/01/2008</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.4532548490281976</v>
+        <v>0.3467491695790255</v>
       </c>
     </row>
     <row r="56">
@@ -1268,11 +1268,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>01/01/2011</t>
+          <t>01/01/2009</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.3123523449870334</v>
+        <v>0.4085367151094751</v>
       </c>
     </row>
     <row r="57">
@@ -1283,11 +1283,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
+          <t>01/01/2010</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1.385008639330851</v>
+        <v>0.4532548490281976</v>
       </c>
     </row>
     <row r="58">
@@ -1298,11 +1298,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
+          <t>01/01/2011</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1.492646399277098</v>
+        <v>0.3123523449870334</v>
       </c>
     </row>
     <row r="59">
@@ -1313,11 +1313,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
+          <t>01/01/2012</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1.346030902059082</v>
+        <v>1.385008639330851</v>
       </c>
     </row>
     <row r="60">
@@ -1328,11 +1328,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
+          <t>01/01/2013</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.9489994144273937</v>
+        <v>1.492646399277098</v>
       </c>
     </row>
     <row r="61">
@@ -1343,11 +1343,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
+          <t>01/01/2014</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.8865412141247279</v>
+        <v>1.346030902059082</v>
       </c>
     </row>
     <row r="62">
@@ -1358,11 +1358,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.7644810349897089</v>
+        <v>0.9489994144273937</v>
       </c>
     </row>
     <row r="63">
@@ -1373,11 +1373,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.7216102118305355</v>
+        <v>0.8865412141247279</v>
       </c>
     </row>
     <row r="64">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.6647873498486689</v>
+        <v>0.7644810349897089</v>
       </c>
     </row>
     <row r="65">
@@ -1403,11 +1403,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.7509610323321583</v>
+        <v>0.7216124650668998</v>
       </c>
     </row>
     <row r="66">
@@ -1418,11 +1418,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.8699269782921861</v>
+        <v>0.6650468019211764</v>
       </c>
     </row>
     <row r="67">
@@ -1433,11 +1433,56 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>0.7519397426027848</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>0.8725628497491614</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
           <t>01/01/2022</t>
         </is>
       </c>
-      <c r="C67" t="n">
-        <v>0.7152851490881019</v>
+      <c r="C69" t="n">
+        <v>0.9812372147795632</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>0.3053398335988244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update arquivos xlsx e alguns scripts específicos
</commit_message>
<xml_diff>
--- a/Data/g18.4.xlsx
+++ b/Data/g18.4.xlsx
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1.136594498038898</v>
+        <v>1.136561060254474</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.9802234811451884</v>
+        <v>0.9801727885739097</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.065265304870053</v>
+        <v>1.065143301680852</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.088090471808203</v>
+        <v>1.087999222857698</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.9289493313642693</v>
+        <v>0.9289168935667048</v>
       </c>
     </row>
     <row r="25">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1.256442541710183</v>
+        <v>1.256485985418618</v>
       </c>
     </row>
     <row r="44">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1.069206783970344</v>
+        <v>1.069272285263012</v>
       </c>
     </row>
     <row r="45">
@@ -1107,7 +1107,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1.166777397737805</v>
+        <v>1.166151053012735</v>
       </c>
     </row>
     <row r="46">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1.208486676710563</v>
+        <v>1.208059761243083</v>
       </c>
     </row>
     <row r="47">
@@ -1137,7 +1137,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1.0004774749174</v>
+        <v>1.00016250814436</v>
       </c>
     </row>
     <row r="48">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.6653630211826647</v>
+        <v>0.6652938879862974</v>
       </c>
     </row>
     <row r="67">
@@ -1437,7 +1437,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.7523026084511003</v>
+        <v>0.75218241541942</v>
       </c>
     </row>
     <row r="68">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.873474070102373</v>
+        <v>0.8731583277241791</v>
       </c>
     </row>
     <row r="69">
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.9825075367110765</v>
+        <v>0.9822359006765974</v>
       </c>
     </row>
     <row r="70">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.9002553232488679</v>
+        <v>0.8999978929815214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>